<commit_message>
added STL and LGW to leaflet
</commit_message>
<xml_diff>
--- a/data/derived_data/iptds_site_species_coverage_sy2023_20240321.xlsx
+++ b/data/derived_data/iptds_site_species_coverage_sy2023_20240321.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mikea\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git\SnakeR_IPTDS\data\derived_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F74CCCCF-F3D3-4AE7-856D-2DC18D563E31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2D13149-1BA1-4AF2-810F-E752AE6DDEA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="in" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="205">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="207">
   <si>
     <t>site_code</t>
   </si>
@@ -651,6 +651,12 @@
   </si>
   <si>
     <t>chinook_site</t>
+  </si>
+  <si>
+    <t>BED</t>
+  </si>
+  <si>
+    <t>Bedrock Creek Seasonal IPTDS</t>
   </si>
 </sst>
 </file>
@@ -1494,10 +1500,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D101"/>
+  <dimension ref="A1:D102"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1789,10 +1795,10 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>41</v>
+        <v>205</v>
       </c>
       <c r="B21" t="s">
-        <v>42</v>
+        <v>206</v>
       </c>
       <c r="C21" s="1" t="b">
         <v>1</v>
@@ -1803,24 +1809,24 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B22" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C22" s="1" t="b">
         <v>1</v>
       </c>
       <c r="D22" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B23" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C23" s="1" t="b">
         <v>1</v>
@@ -1831,10 +1837,10 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B24" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C24" s="1" t="b">
         <v>1</v>
@@ -1845,38 +1851,38 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B25" t="s">
-        <v>50</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D25" s="1" t="s">
-        <v>4</v>
+        <v>48</v>
+      </c>
+      <c r="C25" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="D25" s="1" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B26" t="s">
-        <v>52</v>
-      </c>
-      <c r="C26" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="D26" s="1" t="b">
-        <v>1</v>
+        <v>50</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B27" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C27" s="1" t="b">
         <v>1</v>
@@ -1887,10 +1893,10 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B28" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C28" s="1" t="b">
         <v>1</v>
@@ -1901,10 +1907,10 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B29" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C29" s="1" t="b">
         <v>1</v>
@@ -1915,10 +1921,10 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B30" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C30" s="1" t="b">
         <v>1</v>
@@ -1929,10 +1935,10 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B31" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C31" s="1" t="b">
         <v>1</v>
@@ -1943,10 +1949,10 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B32" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C32" s="1" t="b">
         <v>1</v>
@@ -1957,10 +1963,10 @@
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B33" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C33" s="1" t="b">
         <v>1</v>
@@ -1971,10 +1977,10 @@
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B34" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C34" s="1" t="b">
         <v>1</v>
@@ -1985,10 +1991,10 @@
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B35" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C35" s="1" t="b">
         <v>1</v>
@@ -1999,10 +2005,10 @@
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B36" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C36" s="1" t="b">
         <v>1</v>
@@ -2013,10 +2019,10 @@
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B37" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C37" s="1" t="b">
         <v>1</v>
@@ -2027,10 +2033,10 @@
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B38" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C38" s="1" t="b">
         <v>1</v>
@@ -2041,10 +2047,10 @@
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B39" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C39" s="1" t="b">
         <v>1</v>
@@ -2055,10 +2061,10 @@
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B40" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C40" s="1" t="b">
         <v>1</v>
@@ -2069,10 +2075,10 @@
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B41" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C41" s="1" t="b">
         <v>1</v>
@@ -2083,10 +2089,10 @@
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B42" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C42" s="1" t="b">
         <v>1</v>
@@ -2097,10 +2103,10 @@
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B43" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C43" s="1" t="b">
         <v>1</v>
@@ -2111,10 +2117,10 @@
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B44" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C44" s="1" t="b">
         <v>1</v>
@@ -2125,10 +2131,10 @@
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B45" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C45" s="1" t="b">
         <v>1</v>
@@ -2139,38 +2145,38 @@
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B46" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C46" s="1" t="b">
         <v>1</v>
       </c>
       <c r="D46" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B47" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C47" s="1" t="b">
         <v>1</v>
       </c>
       <c r="D47" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B48" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C48" s="1" t="b">
         <v>1</v>
@@ -2181,10 +2187,10 @@
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B49" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C49" s="1" t="b">
         <v>1</v>
@@ -2195,10 +2201,10 @@
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B50" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C50" s="1" t="b">
         <v>1</v>
@@ -2209,10 +2215,10 @@
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B51" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C51" s="1" t="b">
         <v>1</v>
@@ -2223,10 +2229,10 @@
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B52" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C52" s="1" t="b">
         <v>1</v>
@@ -2237,13 +2243,13 @@
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B53" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C53" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D53" s="1" t="b">
         <v>1</v>
@@ -2251,13 +2257,13 @@
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B54" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C54" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D54" s="1" t="b">
         <v>1</v>
@@ -2265,10 +2271,10 @@
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B55" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C55" s="1" t="b">
         <v>1</v>
@@ -2279,10 +2285,10 @@
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B56" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C56" s="1" t="b">
         <v>1</v>
@@ -2293,10 +2299,10 @@
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B57" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C57" s="1" t="b">
         <v>1</v>
@@ -2307,10 +2313,10 @@
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B58" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C58" s="1" t="b">
         <v>1</v>
@@ -2321,10 +2327,10 @@
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B59" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C59" s="1" t="b">
         <v>1</v>
@@ -2335,10 +2341,10 @@
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B60" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C60" s="1" t="b">
         <v>1</v>
@@ -2349,10 +2355,10 @@
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B61" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C61" s="1" t="b">
         <v>1</v>
@@ -2363,10 +2369,10 @@
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B62" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C62" s="1" t="b">
         <v>1</v>
@@ -2377,10 +2383,10 @@
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B63" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C63" s="1" t="b">
         <v>1</v>
@@ -2391,66 +2397,66 @@
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B64" t="s">
-        <v>128</v>
-      </c>
-      <c r="C64" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D64" s="1" t="s">
-        <v>4</v>
+        <v>126</v>
+      </c>
+      <c r="C64" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="D64" s="1" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B65" t="s">
-        <v>130</v>
-      </c>
-      <c r="C65" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="D65" s="1" t="b">
-        <v>1</v>
+        <v>128</v>
+      </c>
+      <c r="C65" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D65" s="1" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B66" t="s">
-        <v>132</v>
-      </c>
-      <c r="C66" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D66" s="1" t="s">
-        <v>4</v>
+        <v>130</v>
+      </c>
+      <c r="C66" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="D66" s="1" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B67" t="s">
-        <v>134</v>
-      </c>
-      <c r="C67" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="D67" s="1" t="b">
-        <v>1</v>
+        <v>132</v>
+      </c>
+      <c r="C67" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D67" s="1" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B68" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C68" s="1" t="b">
         <v>1</v>
@@ -2461,10 +2467,10 @@
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B69" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C69" s="1" t="b">
         <v>1</v>
@@ -2475,10 +2481,10 @@
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B70" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="C70" s="1" t="b">
         <v>1</v>
@@ -2489,10 +2495,10 @@
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B71" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="C71" s="1" t="b">
         <v>1</v>
@@ -2503,10 +2509,10 @@
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B72" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C72" s="1" t="b">
         <v>1</v>
@@ -2517,10 +2523,10 @@
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B73" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C73" s="1" t="b">
         <v>1</v>
@@ -2531,10 +2537,10 @@
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B74" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C74" s="1" t="b">
         <v>1</v>
@@ -2545,24 +2551,24 @@
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B75" t="s">
-        <v>150</v>
-      </c>
-      <c r="C75" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D75" s="1" t="s">
-        <v>4</v>
+        <v>148</v>
+      </c>
+      <c r="C75" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="D75" s="1" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B76" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C76" s="1" t="s">
         <v>4</v>
@@ -2573,38 +2579,38 @@
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B77" t="s">
-        <v>154</v>
-      </c>
-      <c r="C77" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="D77" s="1" t="b">
-        <v>1</v>
+        <v>152</v>
+      </c>
+      <c r="C77" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D77" s="1" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="B78" t="s">
-        <v>156</v>
-      </c>
-      <c r="C78" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D78" s="1" t="s">
-        <v>4</v>
+        <v>154</v>
+      </c>
+      <c r="C78" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="D78" s="1" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B79" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C79" s="1" t="s">
         <v>4</v>
@@ -2615,24 +2621,24 @@
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="B80" t="s">
-        <v>160</v>
-      </c>
-      <c r="C80" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="D80" s="1" t="b">
-        <v>1</v>
+        <v>158</v>
+      </c>
+      <c r="C80" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D80" s="1" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="B81" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="C81" s="1" t="b">
         <v>1</v>
@@ -2643,38 +2649,38 @@
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="B82" t="s">
-        <v>164</v>
-      </c>
-      <c r="C82" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D82" s="1" t="s">
-        <v>4</v>
+        <v>162</v>
+      </c>
+      <c r="C82" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="D82" s="1" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B83" t="s">
-        <v>166</v>
-      </c>
-      <c r="C83" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="D83" s="1" t="b">
-        <v>1</v>
+        <v>164</v>
+      </c>
+      <c r="C83" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D83" s="1" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B84" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="C84" s="1" t="b">
         <v>1</v>
@@ -2685,10 +2691,10 @@
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B85" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="C85" s="1" t="b">
         <v>1</v>
@@ -2699,38 +2705,38 @@
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B86" t="s">
-        <v>172</v>
-      </c>
-      <c r="C86" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D86" s="1" t="s">
-        <v>4</v>
+        <v>170</v>
+      </c>
+      <c r="C86" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="D86" s="1" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B87" t="s">
-        <v>174</v>
-      </c>
-      <c r="C87" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="D87" s="1" t="b">
-        <v>1</v>
+        <v>172</v>
+      </c>
+      <c r="C87" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D87" s="1" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="B88" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="C88" s="1" t="b">
         <v>1</v>
@@ -2741,10 +2747,10 @@
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="B89" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="C89" s="1" t="b">
         <v>1</v>
@@ -2755,41 +2761,41 @@
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="B90" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="C90" s="1" t="b">
         <v>1</v>
       </c>
       <c r="D90" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B91" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="C91" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="D91" s="1" t="b">
         <v>0</v>
-      </c>
-      <c r="D91" s="1" t="b">
-        <v>1</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="B92" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="C92" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D92" s="1" t="b">
         <v>1</v>
@@ -2797,10 +2803,10 @@
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="B93" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="C93" s="1" t="b">
         <v>1</v>
@@ -2811,24 +2817,24 @@
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="B94" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C94" s="1" t="b">
         <v>1</v>
       </c>
       <c r="D94" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="B95" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="C95" s="1" t="b">
         <v>1</v>
@@ -2839,24 +2845,24 @@
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="B96" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="C96" s="1" t="b">
         <v>1</v>
       </c>
       <c r="D96" s="1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A97" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="B97" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="C97" s="1" t="b">
         <v>1</v>
@@ -2867,24 +2873,24 @@
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="B98" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="C98" s="1" t="b">
         <v>1</v>
       </c>
       <c r="D98" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A99" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="B99" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="C99" s="1" t="b">
         <v>1</v>
@@ -2895,29 +2901,43 @@
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A100" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="B100" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="C100" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="D100" s="1" t="b">
         <v>0</v>
-      </c>
-      <c r="D100" s="1" t="b">
-        <v>1</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A101" t="s">
+        <v>199</v>
+      </c>
+      <c r="B101" t="s">
+        <v>200</v>
+      </c>
+      <c r="C101" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D101" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A102" t="s">
         <v>201</v>
       </c>
-      <c r="B101" t="s">
+      <c r="B102" t="s">
         <v>202</v>
       </c>
-      <c r="C101" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="D101" s="1" t="b">
+      <c r="C102" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="D102" s="1" t="b">
         <v>1</v>
       </c>
     </row>

</xml_diff>